<commit_message>
Them test case dang nhap
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Operation Test" sheetId="15" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Operation Test'!$A$1:$K$56</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Overview!$A$1:$Y$37</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="88">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -195,6 +195,9 @@
     <t>Hiển thị được kết quả đăng kí tài khoản, đăng nhập tài khoản đó thành công</t>
   </si>
   <si>
+    <t>Hoang</t>
+  </si>
+  <si>
     <t>1.2-1</t>
   </si>
   <si>
@@ -213,6 +216,24 @@
     <t>2.2-1</t>
   </si>
   <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>Chức năng của khách sạn</t>
+  </si>
+  <si>
+    <t>Đăng nhập</t>
+  </si>
+  <si>
+    <t>Đăng nhập thành công</t>
+  </si>
+  <si>
+    <t>3.1-1</t>
+  </si>
+  <si>
+    <t>3.2-1</t>
+  </si>
+  <si>
     <t>Phần mềm đặt khách sạn</t>
   </si>
   <si>
@@ -262,6 +283,18 @@
   </si>
   <si>
     <t>1. Phần mềm hiển thị con đường ngắn nhất để đến bãi đỗ xe</t>
+  </si>
+  <si>
+    <t>Đăng nhập 2</t>
+  </si>
+  <si>
+    <t>1. Khách hàng đăng nhập thông tin đúng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Khách hàng nhập sai thông tin </t>
+  </si>
+  <si>
+    <t>Đăng nhập thất bại</t>
   </si>
 </sst>
 </file>
@@ -754,7 +787,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1047,6 +1080,12 @@
     <xf numFmtId="49" fontId="18" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1110,7 +1149,13 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1652,7 +1697,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="75" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F9" s="75"/>
       <c r="G9" s="28"/>
@@ -2470,10 +2515,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor indexed="31"/>
   </sheetPr>
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:K82"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:K82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -2490,7 +2535,7 @@
         <v>19</v>
       </c>
       <c r="B1" s="75" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="C1" s="75"/>
       <c r="D1" s="75"/>
@@ -2549,7 +2594,7 @@
         <v>29</v>
       </c>
       <c r="I3" s="99">
-        <f>COUNTIF(H2:H785,"Untested")</f>
+        <f>COUNTIF(H2:H798,"Untested")</f>
         <v>0</v>
       </c>
       <c r="J3" s="86" t="s">
@@ -2648,22 +2693,22 @@
       <c r="A9" s="48">
         <v>1</v>
       </c>
-      <c r="B9" s="134" t="s">
+      <c r="B9" s="136" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="135"/>
-      <c r="D9" s="128" t="s">
+      <c r="C9" s="137"/>
+      <c r="D9" s="130" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="129"/>
-      <c r="F9" s="140" t="s">
+      <c r="E9" s="131"/>
+      <c r="F9" s="142" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="141"/>
-      <c r="H9" s="126" t="s">
+      <c r="G9" s="143"/>
+      <c r="H9" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="127"/>
+      <c r="I9" s="129"/>
       <c r="J9" s="48"/>
       <c r="K9" s="122"/>
     </row>
@@ -2671,12 +2716,12 @@
       <c r="A10" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="136"/>
-      <c r="C10" s="137"/>
-      <c r="D10" s="130"/>
-      <c r="E10" s="131"/>
-      <c r="F10" s="142"/>
-      <c r="G10" s="143"/>
+      <c r="B10" s="138"/>
+      <c r="C10" s="139"/>
+      <c r="D10" s="132"/>
+      <c r="E10" s="133"/>
+      <c r="F10" s="144"/>
+      <c r="G10" s="145"/>
       <c r="H10" s="115" t="s">
         <v>42</v>
       </c>
@@ -2692,14 +2737,14 @@
       <c r="A11" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="136"/>
-      <c r="C11" s="137"/>
-      <c r="D11" s="130"/>
-      <c r="E11" s="131"/>
-      <c r="F11" s="142"/>
-      <c r="G11" s="143"/>
+      <c r="B11" s="138"/>
+      <c r="C11" s="139"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="133"/>
+      <c r="F11" s="144"/>
+      <c r="G11" s="145"/>
       <c r="H11" s="50" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I11" s="50"/>
       <c r="J11" s="48"/>
@@ -2709,12 +2754,12 @@
       <c r="A12" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="136"/>
-      <c r="C12" s="137"/>
-      <c r="D12" s="130"/>
-      <c r="E12" s="131"/>
-      <c r="F12" s="142"/>
-      <c r="G12" s="143"/>
+      <c r="B12" s="138"/>
+      <c r="C12" s="139"/>
+      <c r="D12" s="132"/>
+      <c r="E12" s="133"/>
+      <c r="F12" s="144"/>
+      <c r="G12" s="145"/>
       <c r="H12" s="115" t="s">
         <v>47</v>
       </c>
@@ -2728,12 +2773,12 @@
       <c r="A13" s="51">
         <v>111</v>
       </c>
-      <c r="B13" s="138"/>
-      <c r="C13" s="139"/>
-      <c r="D13" s="132"/>
-      <c r="E13" s="133"/>
-      <c r="F13" s="144"/>
-      <c r="G13" s="145"/>
+      <c r="B13" s="140"/>
+      <c r="C13" s="141"/>
+      <c r="D13" s="134"/>
+      <c r="E13" s="135"/>
+      <c r="F13" s="146"/>
+      <c r="G13" s="147"/>
       <c r="H13" s="52">
         <v>43389</v>
       </c>
@@ -2745,22 +2790,22 @@
       <c r="A14" s="48">
         <v>2</v>
       </c>
-      <c r="B14" s="134" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="135"/>
-      <c r="D14" s="128" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="129"/>
-      <c r="F14" s="140" t="s">
-        <v>65</v>
-      </c>
-      <c r="G14" s="141"/>
-      <c r="H14" s="126" t="s">
+      <c r="B14" s="136" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="137"/>
+      <c r="D14" s="130" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="131"/>
+      <c r="F14" s="142" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="143"/>
+      <c r="H14" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="127"/>
+      <c r="I14" s="129"/>
       <c r="J14" s="48"/>
       <c r="K14" s="122"/>
     </row>
@@ -2768,12 +2813,12 @@
       <c r="A15" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="136"/>
-      <c r="C15" s="137"/>
-      <c r="D15" s="130"/>
-      <c r="E15" s="131"/>
-      <c r="F15" s="142"/>
-      <c r="G15" s="143"/>
+      <c r="B15" s="138"/>
+      <c r="C15" s="139"/>
+      <c r="D15" s="132"/>
+      <c r="E15" s="133"/>
+      <c r="F15" s="144"/>
+      <c r="G15" s="145"/>
       <c r="H15" s="115" t="s">
         <v>42</v>
       </c>
@@ -2787,16 +2832,16 @@
     </row>
     <row r="16" spans="1:11" ht="10.5" customHeight="1">
       <c r="A16" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="136"/>
-      <c r="C16" s="137"/>
-      <c r="D16" s="130"/>
-      <c r="E16" s="131"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="143"/>
+        <v>55</v>
+      </c>
+      <c r="B16" s="138"/>
+      <c r="C16" s="139"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="145"/>
       <c r="H16" s="50" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I16" s="50"/>
       <c r="J16" s="48"/>
@@ -2806,12 +2851,12 @@
       <c r="A17" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="136"/>
-      <c r="C17" s="137"/>
-      <c r="D17" s="130"/>
-      <c r="E17" s="131"/>
-      <c r="F17" s="142"/>
-      <c r="G17" s="143"/>
+      <c r="B17" s="138"/>
+      <c r="C17" s="139"/>
+      <c r="D17" s="132"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="144"/>
+      <c r="G17" s="145"/>
       <c r="H17" s="115" t="s">
         <v>47</v>
       </c>
@@ -2825,12 +2870,12 @@
       <c r="A18" s="51">
         <v>121</v>
       </c>
-      <c r="B18" s="138"/>
-      <c r="C18" s="139"/>
-      <c r="D18" s="132"/>
-      <c r="E18" s="133"/>
-      <c r="F18" s="144"/>
-      <c r="G18" s="145"/>
+      <c r="B18" s="140"/>
+      <c r="C18" s="141"/>
+      <c r="D18" s="134"/>
+      <c r="E18" s="135"/>
+      <c r="F18" s="146"/>
+      <c r="G18" s="147"/>
       <c r="H18" s="52">
         <v>43389</v>
       </c>
@@ -2854,10 +2899,10 @@
         <v>36</v>
       </c>
       <c r="G19" s="121"/>
-      <c r="H19" s="125" t="s">
+      <c r="H19" s="127" t="s">
         <v>37</v>
       </c>
-      <c r="I19" s="125"/>
+      <c r="I19" s="127"/>
       <c r="J19" s="116" t="s">
         <v>38</v>
       </c>
@@ -2869,22 +2914,22 @@
       <c r="A20" s="48">
         <v>3</v>
       </c>
-      <c r="B20" s="134" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="135"/>
-      <c r="D20" s="128" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="129"/>
-      <c r="F20" s="140" t="s">
-        <v>67</v>
-      </c>
-      <c r="G20" s="141"/>
-      <c r="H20" s="126" t="s">
+      <c r="B20" s="136" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="137"/>
+      <c r="D20" s="130" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="131"/>
+      <c r="F20" s="142" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="143"/>
+      <c r="H20" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="I20" s="127"/>
+      <c r="I20" s="129"/>
       <c r="J20" s="48"/>
       <c r="K20" s="122"/>
     </row>
@@ -2892,12 +2937,12 @@
       <c r="A21" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="136"/>
-      <c r="C21" s="137"/>
-      <c r="D21" s="130"/>
-      <c r="E21" s="131"/>
-      <c r="F21" s="142"/>
-      <c r="G21" s="143"/>
+      <c r="B21" s="138"/>
+      <c r="C21" s="139"/>
+      <c r="D21" s="132"/>
+      <c r="E21" s="133"/>
+      <c r="F21" s="144"/>
+      <c r="G21" s="145"/>
       <c r="H21" s="115" t="s">
         <v>42</v>
       </c>
@@ -2911,16 +2956,16 @@
     </row>
     <row r="22" spans="1:11" ht="10.5" customHeight="1">
       <c r="A22" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="136"/>
-      <c r="C22" s="137"/>
-      <c r="D22" s="130"/>
-      <c r="E22" s="131"/>
-      <c r="F22" s="142"/>
-      <c r="G22" s="143"/>
+        <v>56</v>
+      </c>
+      <c r="B22" s="138"/>
+      <c r="C22" s="139"/>
+      <c r="D22" s="132"/>
+      <c r="E22" s="133"/>
+      <c r="F22" s="144"/>
+      <c r="G22" s="145"/>
       <c r="H22" s="50" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I22" s="50"/>
       <c r="J22" s="48"/>
@@ -2930,12 +2975,12 @@
       <c r="A23" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="136"/>
-      <c r="C23" s="137"/>
-      <c r="D23" s="130"/>
-      <c r="E23" s="131"/>
-      <c r="F23" s="142"/>
-      <c r="G23" s="143"/>
+      <c r="B23" s="138"/>
+      <c r="C23" s="139"/>
+      <c r="D23" s="132"/>
+      <c r="E23" s="133"/>
+      <c r="F23" s="144"/>
+      <c r="G23" s="145"/>
       <c r="H23" s="115" t="s">
         <v>47</v>
       </c>
@@ -2949,12 +2994,12 @@
       <c r="A24" s="51">
         <v>131</v>
       </c>
-      <c r="B24" s="138"/>
-      <c r="C24" s="139"/>
-      <c r="D24" s="132"/>
-      <c r="E24" s="133"/>
-      <c r="F24" s="144"/>
-      <c r="G24" s="145"/>
+      <c r="B24" s="140"/>
+      <c r="C24" s="141"/>
+      <c r="D24" s="134"/>
+      <c r="E24" s="135"/>
+      <c r="F24" s="146"/>
+      <c r="G24" s="147"/>
       <c r="H24" s="52">
         <v>43389</v>
       </c>
@@ -2978,10 +3023,10 @@
         <v>36</v>
       </c>
       <c r="G25" s="121"/>
-      <c r="H25" s="125" t="s">
+      <c r="H25" s="127" t="s">
         <v>37</v>
       </c>
-      <c r="I25" s="125"/>
+      <c r="I25" s="127"/>
       <c r="J25" s="116" t="s">
         <v>38</v>
       </c>
@@ -2993,22 +3038,22 @@
       <c r="A26" s="48">
         <v>4</v>
       </c>
-      <c r="B26" s="134" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="135"/>
-      <c r="D26" s="128" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="129"/>
-      <c r="F26" s="140" t="s">
-        <v>71</v>
-      </c>
-      <c r="G26" s="141"/>
-      <c r="H26" s="126" t="s">
+      <c r="B26" s="136" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="137"/>
+      <c r="D26" s="130" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="131"/>
+      <c r="F26" s="142" t="s">
+        <v>78</v>
+      </c>
+      <c r="G26" s="143"/>
+      <c r="H26" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="I26" s="127"/>
+      <c r="I26" s="129"/>
       <c r="J26" s="48"/>
       <c r="K26" s="122"/>
     </row>
@@ -3016,12 +3061,12 @@
       <c r="A27" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="136"/>
-      <c r="C27" s="137"/>
-      <c r="D27" s="130"/>
-      <c r="E27" s="131"/>
-      <c r="F27" s="142"/>
-      <c r="G27" s="143"/>
+      <c r="B27" s="138"/>
+      <c r="C27" s="139"/>
+      <c r="D27" s="132"/>
+      <c r="E27" s="133"/>
+      <c r="F27" s="144"/>
+      <c r="G27" s="145"/>
       <c r="H27" s="115" t="s">
         <v>42</v>
       </c>
@@ -3035,16 +3080,16 @@
     </row>
     <row r="28" spans="1:11" ht="10.5" customHeight="1">
       <c r="A28" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="136"/>
-      <c r="C28" s="137"/>
-      <c r="D28" s="130"/>
-      <c r="E28" s="131"/>
-      <c r="F28" s="142"/>
-      <c r="G28" s="143"/>
+        <v>57</v>
+      </c>
+      <c r="B28" s="138"/>
+      <c r="C28" s="139"/>
+      <c r="D28" s="132"/>
+      <c r="E28" s="133"/>
+      <c r="F28" s="144"/>
+      <c r="G28" s="145"/>
       <c r="H28" s="50" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I28" s="50"/>
       <c r="J28" s="48"/>
@@ -3054,12 +3099,12 @@
       <c r="A29" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="136"/>
-      <c r="C29" s="137"/>
-      <c r="D29" s="130"/>
-      <c r="E29" s="131"/>
-      <c r="F29" s="142"/>
-      <c r="G29" s="143"/>
+      <c r="B29" s="138"/>
+      <c r="C29" s="139"/>
+      <c r="D29" s="132"/>
+      <c r="E29" s="133"/>
+      <c r="F29" s="144"/>
+      <c r="G29" s="145"/>
       <c r="H29" s="115" t="s">
         <v>47</v>
       </c>
@@ -3073,12 +3118,12 @@
       <c r="A30" s="51">
         <v>141</v>
       </c>
-      <c r="B30" s="138"/>
-      <c r="C30" s="139"/>
-      <c r="D30" s="132"/>
-      <c r="E30" s="133"/>
-      <c r="F30" s="144"/>
-      <c r="G30" s="145"/>
+      <c r="B30" s="140"/>
+      <c r="C30" s="141"/>
+      <c r="D30" s="134"/>
+      <c r="E30" s="135"/>
+      <c r="F30" s="146"/>
+      <c r="G30" s="147"/>
       <c r="H30" s="52">
         <v>43389</v>
       </c>
@@ -3090,18 +3135,18 @@
       <c r="A31" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="146" t="s">
-        <v>57</v>
-      </c>
-      <c r="C31" s="146"/>
-      <c r="D31" s="119"/>
-      <c r="E31" s="119"/>
-      <c r="F31" s="119"/>
-      <c r="G31" s="119"/>
-      <c r="H31" s="119"/>
-      <c r="I31" s="119"/>
-      <c r="J31" s="119"/>
-      <c r="K31" s="119"/>
+      <c r="B31" s="148" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="149"/>
+      <c r="D31" s="149"/>
+      <c r="E31" s="149"/>
+      <c r="F31" s="149"/>
+      <c r="G31" s="149"/>
+      <c r="H31" s="149"/>
+      <c r="I31" s="149"/>
+      <c r="J31" s="149"/>
+      <c r="K31" s="150"/>
     </row>
     <row r="32" spans="1:11" ht="10.5" customHeight="1">
       <c r="A32" s="115" t="s">
@@ -3119,10 +3164,10 @@
         <v>36</v>
       </c>
       <c r="G32" s="121"/>
-      <c r="H32" s="125" t="s">
+      <c r="H32" s="127" t="s">
         <v>37</v>
       </c>
-      <c r="I32" s="125"/>
+      <c r="I32" s="127"/>
       <c r="J32" s="116" t="s">
         <v>38</v>
       </c>
@@ -3134,22 +3179,22 @@
       <c r="A33" s="48">
         <v>5</v>
       </c>
-      <c r="B33" s="134" t="s">
-        <v>72</v>
-      </c>
-      <c r="C33" s="135"/>
-      <c r="D33" s="128" t="s">
-        <v>73</v>
-      </c>
-      <c r="E33" s="129"/>
-      <c r="F33" s="140" t="s">
-        <v>74</v>
-      </c>
-      <c r="G33" s="141"/>
-      <c r="H33" s="126" t="s">
+      <c r="B33" s="136" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="137"/>
+      <c r="D33" s="130" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="131"/>
+      <c r="F33" s="142" t="s">
+        <v>81</v>
+      </c>
+      <c r="G33" s="143"/>
+      <c r="H33" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="I33" s="127"/>
+      <c r="I33" s="129"/>
       <c r="J33" s="48"/>
       <c r="K33" s="122"/>
     </row>
@@ -3157,12 +3202,12 @@
       <c r="A34" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="136"/>
-      <c r="C34" s="137"/>
-      <c r="D34" s="130"/>
-      <c r="E34" s="131"/>
-      <c r="F34" s="142"/>
-      <c r="G34" s="143"/>
+      <c r="B34" s="138"/>
+      <c r="C34" s="139"/>
+      <c r="D34" s="132"/>
+      <c r="E34" s="133"/>
+      <c r="F34" s="144"/>
+      <c r="G34" s="145"/>
       <c r="H34" s="115" t="s">
         <v>42</v>
       </c>
@@ -3176,16 +3221,16 @@
     </row>
     <row r="35" spans="1:11" ht="10.5" customHeight="1">
       <c r="A35" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="136"/>
-      <c r="C35" s="137"/>
-      <c r="D35" s="130"/>
-      <c r="E35" s="131"/>
-      <c r="F35" s="142"/>
-      <c r="G35" s="143"/>
+        <v>59</v>
+      </c>
+      <c r="B35" s="138"/>
+      <c r="C35" s="139"/>
+      <c r="D35" s="132"/>
+      <c r="E35" s="133"/>
+      <c r="F35" s="144"/>
+      <c r="G35" s="145"/>
       <c r="H35" s="50" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I35" s="50"/>
       <c r="J35" s="48"/>
@@ -3195,12 +3240,12 @@
       <c r="A36" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="136"/>
-      <c r="C36" s="137"/>
-      <c r="D36" s="130"/>
-      <c r="E36" s="131"/>
-      <c r="F36" s="142"/>
-      <c r="G36" s="143"/>
+      <c r="B36" s="138"/>
+      <c r="C36" s="139"/>
+      <c r="D36" s="132"/>
+      <c r="E36" s="133"/>
+      <c r="F36" s="144"/>
+      <c r="G36" s="145"/>
       <c r="H36" s="115" t="s">
         <v>47</v>
       </c>
@@ -3214,12 +3259,12 @@
       <c r="A37" s="51">
         <v>211</v>
       </c>
-      <c r="B37" s="138"/>
-      <c r="C37" s="139"/>
-      <c r="D37" s="132"/>
-      <c r="E37" s="133"/>
-      <c r="F37" s="144"/>
-      <c r="G37" s="145"/>
+      <c r="B37" s="140"/>
+      <c r="C37" s="141"/>
+      <c r="D37" s="134"/>
+      <c r="E37" s="135"/>
+      <c r="F37" s="146"/>
+      <c r="G37" s="147"/>
       <c r="H37" s="52">
         <v>43389</v>
       </c>
@@ -3243,10 +3288,10 @@
         <v>36</v>
       </c>
       <c r="G38" s="121"/>
-      <c r="H38" s="125" t="s">
+      <c r="H38" s="127" t="s">
         <v>37</v>
       </c>
-      <c r="I38" s="125"/>
+      <c r="I38" s="127"/>
       <c r="J38" s="116" t="s">
         <v>38</v>
       </c>
@@ -3258,22 +3303,22 @@
       <c r="A39" s="48">
         <v>6</v>
       </c>
-      <c r="B39" s="134" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="135"/>
-      <c r="D39" s="128" t="s">
-        <v>76</v>
-      </c>
-      <c r="E39" s="129"/>
-      <c r="F39" s="140" t="s">
+      <c r="B39" s="136" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="137"/>
+      <c r="D39" s="130" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="131"/>
+      <c r="F39" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="G39" s="141"/>
-      <c r="H39" s="126" t="s">
+      <c r="G39" s="143"/>
+      <c r="H39" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="I39" s="127"/>
+      <c r="I39" s="129"/>
       <c r="J39" s="48"/>
       <c r="K39" s="122"/>
     </row>
@@ -3281,12 +3326,12 @@
       <c r="A40" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="136"/>
-      <c r="C40" s="137"/>
-      <c r="D40" s="130"/>
-      <c r="E40" s="131"/>
-      <c r="F40" s="142"/>
-      <c r="G40" s="143"/>
+      <c r="B40" s="138"/>
+      <c r="C40" s="139"/>
+      <c r="D40" s="132"/>
+      <c r="E40" s="133"/>
+      <c r="F40" s="144"/>
+      <c r="G40" s="145"/>
       <c r="H40" s="115" t="s">
         <v>42</v>
       </c>
@@ -3300,16 +3345,16 @@
     </row>
     <row r="41" spans="1:11" s="55" customFormat="1">
       <c r="A41" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" s="136"/>
-      <c r="C41" s="137"/>
-      <c r="D41" s="130"/>
-      <c r="E41" s="131"/>
-      <c r="F41" s="142"/>
-      <c r="G41" s="143"/>
+        <v>60</v>
+      </c>
+      <c r="B41" s="138"/>
+      <c r="C41" s="139"/>
+      <c r="D41" s="132"/>
+      <c r="E41" s="133"/>
+      <c r="F41" s="144"/>
+      <c r="G41" s="145"/>
       <c r="H41" s="50" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="I41" s="50"/>
       <c r="J41" s="48"/>
@@ -3319,12 +3364,12 @@
       <c r="A42" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="136"/>
-      <c r="C42" s="137"/>
-      <c r="D42" s="130"/>
-      <c r="E42" s="131"/>
-      <c r="F42" s="142"/>
-      <c r="G42" s="143"/>
+      <c r="B42" s="138"/>
+      <c r="C42" s="139"/>
+      <c r="D42" s="132"/>
+      <c r="E42" s="133"/>
+      <c r="F42" s="144"/>
+      <c r="G42" s="145"/>
       <c r="H42" s="115" t="s">
         <v>47</v>
       </c>
@@ -3338,12 +3383,12 @@
       <c r="A43" s="51">
         <v>211</v>
       </c>
-      <c r="B43" s="138"/>
-      <c r="C43" s="139"/>
-      <c r="D43" s="132"/>
-      <c r="E43" s="133"/>
-      <c r="F43" s="144"/>
-      <c r="G43" s="145"/>
+      <c r="B43" s="140"/>
+      <c r="C43" s="141"/>
+      <c r="D43" s="134"/>
+      <c r="E43" s="135"/>
+      <c r="F43" s="146"/>
+      <c r="G43" s="147"/>
       <c r="H43" s="52">
         <v>43389</v>
       </c>
@@ -3351,99 +3396,383 @@
       <c r="J43" s="53"/>
       <c r="K43" s="124"/>
     </row>
-    <row r="44" spans="1:11" s="55" customFormat="1">
-      <c r="A44" s="59"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="59"/>
-      <c r="K44" s="59"/>
+    <row r="44" spans="1:11" s="55" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A44" s="96" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" s="148" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="149"/>
+      <c r="D44" s="149"/>
+      <c r="E44" s="149"/>
+      <c r="F44" s="149"/>
+      <c r="G44" s="149"/>
+      <c r="H44" s="149"/>
+      <c r="I44" s="149"/>
+      <c r="J44" s="149"/>
+      <c r="K44" s="150"/>
     </row>
     <row r="45" spans="1:11" s="55" customFormat="1">
-      <c r="A45" s="59"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="59"/>
-      <c r="J45" s="59"/>
-      <c r="K45" s="59"/>
-    </row>
-    <row r="46" spans="1:11" s="55" customFormat="1">
-      <c r="A46" s="59"/>
-      <c r="H46" s="59"/>
-      <c r="I46" s="59"/>
-      <c r="J46" s="59"/>
-      <c r="K46" s="59"/>
+      <c r="A45" s="115" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="120" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="121"/>
+      <c r="D45" s="120" t="s">
+        <v>35</v>
+      </c>
+      <c r="E45" s="121"/>
+      <c r="F45" s="120" t="s">
+        <v>36</v>
+      </c>
+      <c r="G45" s="121"/>
+      <c r="H45" s="120" t="s">
+        <v>37</v>
+      </c>
+      <c r="I45" s="121"/>
+      <c r="J45" s="116" t="s">
+        <v>38</v>
+      </c>
+      <c r="K45" s="47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="55" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A46" s="48">
+        <v>7</v>
+      </c>
+      <c r="B46" s="136" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" s="137"/>
+      <c r="D46" s="130" t="s">
+        <v>85</v>
+      </c>
+      <c r="E46" s="131"/>
+      <c r="F46" s="142" t="s">
+        <v>64</v>
+      </c>
+      <c r="G46" s="143"/>
+      <c r="H46" s="128" t="s">
+        <v>8</v>
+      </c>
+      <c r="I46" s="129"/>
+      <c r="J46" s="48"/>
+      <c r="K46" s="122"/>
     </row>
     <row r="47" spans="1:11" s="55" customFormat="1">
-      <c r="A47" s="59"/>
-      <c r="H47" s="59"/>
-      <c r="I47" s="59"/>
-      <c r="J47" s="59"/>
-      <c r="K47" s="59"/>
+      <c r="A47" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="138"/>
+      <c r="C47" s="139"/>
+      <c r="D47" s="132"/>
+      <c r="E47" s="133"/>
+      <c r="F47" s="144"/>
+      <c r="G47" s="145"/>
+      <c r="H47" s="115" t="s">
+        <v>42</v>
+      </c>
+      <c r="I47" s="115" t="s">
+        <v>43</v>
+      </c>
+      <c r="J47" s="115" t="s">
+        <v>44</v>
+      </c>
+      <c r="K47" s="123"/>
     </row>
     <row r="48" spans="1:11" s="55" customFormat="1">
-      <c r="A48" s="59"/>
-      <c r="H48" s="59"/>
-      <c r="I48" s="59"/>
-      <c r="J48" s="59"/>
-      <c r="K48" s="59"/>
+      <c r="A48" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" s="138"/>
+      <c r="C48" s="139"/>
+      <c r="D48" s="132"/>
+      <c r="E48" s="133"/>
+      <c r="F48" s="144"/>
+      <c r="G48" s="145"/>
+      <c r="H48" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="I48" s="50"/>
+      <c r="J48" s="48"/>
+      <c r="K48" s="123"/>
     </row>
     <row r="49" spans="1:11" s="55" customFormat="1">
-      <c r="A49" s="59"/>
-      <c r="H49" s="59"/>
-      <c r="I49" s="59"/>
-      <c r="J49" s="59"/>
-      <c r="K49" s="59"/>
+      <c r="A49" s="115" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="138"/>
+      <c r="C49" s="139"/>
+      <c r="D49" s="132"/>
+      <c r="E49" s="133"/>
+      <c r="F49" s="144"/>
+      <c r="G49" s="145"/>
+      <c r="H49" s="115" t="s">
+        <v>47</v>
+      </c>
+      <c r="I49" s="115" t="s">
+        <v>48</v>
+      </c>
+      <c r="J49" s="115"/>
+      <c r="K49" s="123"/>
     </row>
     <row r="50" spans="1:11" s="55" customFormat="1">
-      <c r="A50" s="59"/>
-      <c r="H50" s="59"/>
-      <c r="I50" s="59"/>
-      <c r="J50" s="59"/>
-      <c r="K50" s="59"/>
+      <c r="A50" s="51">
+        <v>311</v>
+      </c>
+      <c r="B50" s="140"/>
+      <c r="C50" s="141"/>
+      <c r="D50" s="134"/>
+      <c r="E50" s="135"/>
+      <c r="F50" s="146"/>
+      <c r="G50" s="147"/>
+      <c r="H50" s="52">
+        <v>42659</v>
+      </c>
+      <c r="I50" s="52"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="124"/>
     </row>
     <row r="51" spans="1:11" s="55" customFormat="1">
-      <c r="A51" s="59"/>
-      <c r="H51" s="59"/>
-      <c r="I51" s="59"/>
-      <c r="J51" s="59"/>
-      <c r="K51" s="59"/>
-    </row>
-    <row r="52" spans="1:11" s="55" customFormat="1">
-      <c r="A52" s="59"/>
-      <c r="H52" s="59"/>
-      <c r="I52" s="59"/>
-      <c r="J52" s="59"/>
-      <c r="K52" s="59"/>
+      <c r="A51" s="115" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51" s="120" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" s="121"/>
+      <c r="D51" s="120" t="s">
+        <v>35</v>
+      </c>
+      <c r="E51" s="121"/>
+      <c r="F51" s="120" t="s">
+        <v>36</v>
+      </c>
+      <c r="G51" s="121"/>
+      <c r="H51" s="125" t="s">
+        <v>37</v>
+      </c>
+      <c r="I51" s="126"/>
+      <c r="J51" s="116" t="s">
+        <v>38</v>
+      </c>
+      <c r="K51" s="47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" s="55" customFormat="1" ht="10.5" customHeight="1">
+      <c r="A52" s="48">
+        <v>8</v>
+      </c>
+      <c r="B52" s="136" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" s="137"/>
+      <c r="D52" s="130" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" s="131"/>
+      <c r="F52" s="142" t="s">
+        <v>87</v>
+      </c>
+      <c r="G52" s="143"/>
+      <c r="H52" s="128" t="s">
+        <v>8</v>
+      </c>
+      <c r="I52" s="129"/>
+      <c r="J52" s="48"/>
+      <c r="K52" s="122"/>
     </row>
     <row r="53" spans="1:11" s="55" customFormat="1">
-      <c r="A53" s="59"/>
-      <c r="H53" s="59"/>
-      <c r="I53" s="59"/>
-      <c r="J53" s="59"/>
-      <c r="K53" s="59"/>
+      <c r="A53" s="115" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="138"/>
+      <c r="C53" s="139"/>
+      <c r="D53" s="132"/>
+      <c r="E53" s="133"/>
+      <c r="F53" s="144"/>
+      <c r="G53" s="145"/>
+      <c r="H53" s="115" t="s">
+        <v>42</v>
+      </c>
+      <c r="I53" s="115" t="s">
+        <v>43</v>
+      </c>
+      <c r="J53" s="115" t="s">
+        <v>44</v>
+      </c>
+      <c r="K53" s="123"/>
     </row>
     <row r="54" spans="1:11" s="55" customFormat="1">
-      <c r="A54" s="59"/>
-      <c r="H54" s="59"/>
-      <c r="I54" s="59"/>
-      <c r="J54" s="59"/>
-      <c r="K54" s="59"/>
+      <c r="A54" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="138"/>
+      <c r="C54" s="139"/>
+      <c r="D54" s="132"/>
+      <c r="E54" s="133"/>
+      <c r="F54" s="144"/>
+      <c r="G54" s="145"/>
+      <c r="H54" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="I54" s="50"/>
+      <c r="J54" s="48"/>
+      <c r="K54" s="123"/>
     </row>
     <row r="55" spans="1:11" s="55" customFormat="1">
-      <c r="A55" s="59"/>
-      <c r="H55" s="59"/>
-      <c r="I55" s="59"/>
-      <c r="J55" s="59"/>
-      <c r="K55" s="59"/>
+      <c r="A55" s="115" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55" s="138"/>
+      <c r="C55" s="139"/>
+      <c r="D55" s="132"/>
+      <c r="E55" s="133"/>
+      <c r="F55" s="144"/>
+      <c r="G55" s="145"/>
+      <c r="H55" s="115" t="s">
+        <v>47</v>
+      </c>
+      <c r="I55" s="115" t="s">
+        <v>48</v>
+      </c>
+      <c r="J55" s="115"/>
+      <c r="K55" s="123"/>
     </row>
     <row r="56" spans="1:11" s="55" customFormat="1">
-      <c r="A56" s="59"/>
-      <c r="H56" s="59"/>
-      <c r="I56" s="59"/>
-      <c r="J56" s="59"/>
-      <c r="K56" s="59"/>
+      <c r="A56" s="51">
+        <v>321</v>
+      </c>
+      <c r="B56" s="140"/>
+      <c r="C56" s="141"/>
+      <c r="D56" s="134"/>
+      <c r="E56" s="135"/>
+      <c r="F56" s="146"/>
+      <c r="G56" s="147"/>
+      <c r="H56" s="52">
+        <v>43324</v>
+      </c>
+      <c r="I56" s="52"/>
+      <c r="J56" s="53"/>
+      <c r="K56" s="124"/>
+    </row>
+    <row r="57" spans="1:11" s="55" customFormat="1">
+      <c r="A57" s="59"/>
+      <c r="H57" s="59"/>
+      <c r="I57" s="59"/>
+      <c r="J57" s="59"/>
+      <c r="K57" s="59"/>
+    </row>
+    <row r="58" spans="1:11" s="55" customFormat="1">
+      <c r="A58" s="59"/>
+      <c r="H58" s="59"/>
+      <c r="I58" s="59"/>
+      <c r="J58" s="59"/>
+      <c r="K58" s="59"/>
+    </row>
+    <row r="59" spans="1:11" s="55" customFormat="1">
+      <c r="A59" s="59"/>
+      <c r="H59" s="59"/>
+      <c r="I59" s="59"/>
+      <c r="J59" s="59"/>
+      <c r="K59" s="59"/>
+    </row>
+    <row r="60" spans="1:11" s="55" customFormat="1">
+      <c r="A60" s="59"/>
+      <c r="H60" s="59"/>
+      <c r="I60" s="59"/>
+      <c r="J60" s="59"/>
+      <c r="K60" s="59"/>
+    </row>
+    <row r="61" spans="1:11" s="55" customFormat="1">
+      <c r="A61" s="59"/>
+      <c r="H61" s="59"/>
+      <c r="I61" s="59"/>
+      <c r="J61" s="59"/>
+      <c r="K61" s="59"/>
+    </row>
+    <row r="62" spans="1:11" s="55" customFormat="1">
+      <c r="A62" s="59"/>
+      <c r="H62" s="59"/>
+      <c r="I62" s="59"/>
+      <c r="J62" s="59"/>
+      <c r="K62" s="59"/>
+    </row>
+    <row r="63" spans="1:11" s="55" customFormat="1">
+      <c r="A63" s="59"/>
+      <c r="H63" s="59"/>
+      <c r="I63" s="59"/>
+      <c r="J63" s="59"/>
+      <c r="K63" s="59"/>
+    </row>
+    <row r="64" spans="1:11" s="55" customFormat="1">
+      <c r="A64" s="59"/>
+      <c r="H64" s="59"/>
+      <c r="I64" s="59"/>
+      <c r="J64" s="59"/>
+      <c r="K64" s="59"/>
+    </row>
+    <row r="65" spans="1:11" s="55" customFormat="1">
+      <c r="A65" s="59"/>
+      <c r="H65" s="59"/>
+      <c r="I65" s="59"/>
+      <c r="J65" s="59"/>
+      <c r="K65" s="59"/>
+    </row>
+    <row r="66" spans="1:11" s="55" customFormat="1">
+      <c r="A66" s="59"/>
+      <c r="H66" s="59"/>
+      <c r="I66" s="59"/>
+      <c r="J66" s="59"/>
+      <c r="K66" s="59"/>
+    </row>
+    <row r="67" spans="1:11" s="55" customFormat="1">
+      <c r="A67" s="59"/>
+      <c r="H67" s="59"/>
+      <c r="I67" s="59"/>
+      <c r="J67" s="59"/>
+      <c r="K67" s="59"/>
+    </row>
+    <row r="68" spans="1:11" s="55" customFormat="1">
+      <c r="A68" s="59"/>
+      <c r="H68" s="59"/>
+      <c r="I68" s="59"/>
+      <c r="J68" s="59"/>
+      <c r="K68" s="59"/>
+    </row>
+    <row r="69" spans="1:11" s="55" customFormat="1">
+      <c r="A69" s="59"/>
+      <c r="H69" s="59"/>
+      <c r="I69" s="59"/>
+      <c r="J69" s="59"/>
+      <c r="K69" s="59"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
+  <mergeCells count="68">
+    <mergeCell ref="B44:K44"/>
+    <mergeCell ref="K52:K56"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="B52:C56"/>
+    <mergeCell ref="D52:E56"/>
+    <mergeCell ref="F52:G56"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="B46:C50"/>
+    <mergeCell ref="D46:E50"/>
+    <mergeCell ref="F46:G50"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="K46:K50"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
     <mergeCell ref="B39:C43"/>
     <mergeCell ref="D39:E43"/>
     <mergeCell ref="F39:G43"/>

</xml_diff>

<commit_message>
Chinh sua test case dang nhap 1
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -2589,8 +2589,8 @@
   </sheetPr>
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A46" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58:C68"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A43" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="10.5"/>
@@ -3603,7 +3603,7 @@
       <c r="F50" s="145"/>
       <c r="G50" s="146"/>
       <c r="H50" s="53">
-        <v>42659</v>
+        <v>43389</v>
       </c>
       <c r="I50" s="53"/>
       <c r="J50" s="54"/>
@@ -3727,7 +3727,7 @@
       <c r="F56" s="145"/>
       <c r="G56" s="146"/>
       <c r="H56" s="53">
-        <v>43324</v>
+        <v>43389</v>
       </c>
       <c r="I56" s="53"/>
       <c r="J56" s="54"/>
@@ -4148,5 +4148,8 @@
     <oddHeader>&amp;LTest Case Table&amp;CBig Point: &amp;A</oddHeader>
     <oddFooter>&amp;LAI&amp;&amp;T-ART&amp;CLiveSpark Project&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="43" max="10" man="1"/>
+  </rowBreaks>
 </worksheet>
 </file>
</xml_diff>